<commit_message>
updates on keyword modifier
</commit_message>
<xml_diff>
--- a/name_generator/dict/text_components.xlsx
+++ b/name_generator/dict/text_components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox (Personal)/masayuki_kishi/repositories/create_names_v2/name_generator/dict/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox/masayuki_kishi/repositories/create_names_v2/name_generator/dict/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154A8801-9036-C749-9CCE-E189F68FFF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED01527D-2AFA-E048-8E99-8D8F800C1EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="500" windowWidth="27260" windowHeight="20740" activeTab="2" xr2:uid="{1ED5CA03-E3A9-144B-B2A8-9DA0B6C9D845}"/>
+    <workbookView xWindow="1540" yWindow="500" windowWidth="27260" windowHeight="16400" activeTab="2" xr2:uid="{1ED5CA03-E3A9-144B-B2A8-9DA0B6C9D845}"/>
   </bookViews>
   <sheets>
     <sheet name="prefixes" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6310" uniqueCount="1222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6311" uniqueCount="1222">
   <si>
     <t>examples</t>
   </si>
@@ -8532,8 +8532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982F055C-371C-1C44-9096-80FAA8E0A3D5}">
   <dimension ref="A1:H415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
-      <selection activeCell="H236" sqref="H236"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10086,7 +10086,9 @@
         <v>533</v>
       </c>
       <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
+      <c r="H70" s="3" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="3">

</xml_diff>